<commit_message>
Add: CalculateLands function, added dictionarties
</commit_message>
<xml_diff>
--- a/Mockups/data.xlsx
+++ b/Mockups/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Dot Net\LandDistribution\Mockups\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF409079-B04B-46EA-8090-6FB76952A754}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF49800B-BA43-48EC-986E-DF437285D753}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{EA124772-A9D3-4F2D-8ADD-97547CD68404}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8880" xr2:uid="{EA124772-A9D3-4F2D-8ADD-97547CD68404}"/>
   </bookViews>
   <sheets>
     <sheet name="גיליון1" sheetId="1" r:id="rId1"/>
@@ -35,15 +35,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>שטחים (שווים)</t>
+    <t>שם שטח</t>
   </si>
   <si>
-    <t>קבוצות (אחוזים)</t>
+    <t>מספר קבוצה</t>
   </si>
   <si>
-    <t>קבוצה</t>
+    <t>אחוז קבוצה</t>
+  </si>
+  <si>
+    <t>אחוז שטח</t>
   </si>
 </sst>
 </file>
@@ -395,30 +398,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DD81EF3-DC64-4C5F-BE4A-7B65EEFC85D1}">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q6" sqref="Q6"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.8984375" customWidth="1"/>
-    <col min="3" max="3" width="11.19921875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="15.8984375" customWidth="1"/>
+    <col min="4" max="4" width="11.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
         <v>2</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -426,10 +433,13 @@
         <v>20</v>
       </c>
       <c r="C2">
-        <v>2.161</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>2.161</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -437,10 +447,13 @@
         <v>16</v>
       </c>
       <c r="C3">
-        <v>2.161</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>2.161</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -448,10 +461,13 @@
         <v>5</v>
       </c>
       <c r="C4">
-        <v>2.161</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>2.161</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -459,10 +475,13 @@
         <v>2</v>
       </c>
       <c r="C5">
-        <v>2.161</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <v>2.161</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -470,10 +489,13 @@
         <v>17.2</v>
       </c>
       <c r="C6">
-        <v>2.161</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="D6">
+        <v>2.161</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -481,10 +503,13 @@
         <v>15</v>
       </c>
       <c r="C7">
-        <v>2.161</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="D7">
+        <v>2.161</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -492,10 +517,13 @@
         <v>4</v>
       </c>
       <c r="C8">
-        <v>2.161</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="D8">
+        <v>2.161</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -503,10 +531,13 @@
         <v>3</v>
       </c>
       <c r="C9">
-        <v>2.161</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="D9">
+        <v>2.161</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -514,10 +545,13 @@
         <v>2</v>
       </c>
       <c r="C10">
-        <v>2.161</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="D10">
+        <v>2.161</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -525,10 +559,13 @@
         <v>3</v>
       </c>
       <c r="C11">
-        <v>2.161</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="D11">
+        <v>2.161</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -536,10 +573,13 @@
         <v>7</v>
       </c>
       <c r="C12">
-        <v>2.161</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+      <c r="D12">
+        <v>2.161</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -547,10 +587,13 @@
         <v>2</v>
       </c>
       <c r="C13">
-        <v>2.161</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="D13">
+        <v>2.161</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -558,6 +601,33 @@
         <v>3.8</v>
       </c>
       <c r="C14">
+        <v>13</v>
+      </c>
+      <c r="D14">
+        <v>2.161</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C15">
+        <v>14</v>
+      </c>
+      <c r="D15">
+        <v>2.161</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C16">
+        <v>15</v>
+      </c>
+      <c r="D16">
+        <v>2.161</v>
+      </c>
+    </row>
+    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C17">
+        <v>16</v>
+      </c>
+      <c r="D17">
         <v>2.161</v>
       </c>
     </row>

</xml_diff>